<commit_message>
update of pin numbering again...
</commit_message>
<xml_diff>
--- a/Pofo.xlsx
+++ b/Pofo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="976" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="76">
   <si>
     <t xml:space="preserve">x</t>
   </si>
@@ -180,19 +180,67 @@
     <t xml:space="preserve">Alt</t>
   </si>
   <si>
+    <t xml:space="preserve">PD7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PE6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF4</t>
+  </si>
+  <si>
     <t xml:space="preserve">21</t>
   </si>
   <si>
+    <t xml:space="preserve">PF5</t>
+  </si>
+  <si>
     <t xml:space="preserve">20</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
+    <t xml:space="preserve">PF6</t>
+  </si>
+  <si>
     <t xml:space="preserve">19</t>
   </si>
   <si>
     <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF7</t>
   </si>
   <si>
     <t xml:space="preserve">18</t>
@@ -307,12 +355,12 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N13" activeCellId="0" sqref="N13"/>
+      <selection pane="topLeft" activeCell="N13" activeCellId="1" sqref="E:E N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="4.60728744939271"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="4.49797570850202"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,268 +1013,321 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E:E"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="5.67611336032389"/>
+    <col collapsed="false" hidden="false" max="10" min="1" style="1" width="5.67611336032389"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="5.67611336032389"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="5.67611336032389"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0"/>
-      <c r="B1" s="1" t="n">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0"/>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0"/>
+      <c r="C2" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="D2" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="E2" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="I2" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="J2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>4</v>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="C6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="0"/>
-      <c r="C6" s="1" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="0"/>
+      <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="0"/>
-      <c r="F7" s="1" t="s">
+      <c r="I8" s="0"/>
+      <c r="J8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="0"/>
-      <c r="F8" s="1" t="s">
+      <c r="I9" s="0"/>
+      <c r="J9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1248,7 +1349,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E:E A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Finally got tmk programmed, it enumerates but doesn't work...
</commit_message>
<xml_diff>
--- a/Pofo.xlsx
+++ b/Pofo.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="78">
   <si>
     <t xml:space="preserve">x</t>
   </si>
@@ -231,6 +231,9 @@
     <t xml:space="preserve">2</t>
   </si>
   <si>
+    <t xml:space="preserve">Ö</t>
+  </si>
+  <si>
     <t xml:space="preserve">PF6</t>
   </si>
   <si>
@@ -238,6 +241,9 @@
   </si>
   <si>
     <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'</t>
   </si>
   <si>
     <t xml:space="preserve">PF7</t>
@@ -360,7 +366,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="4.49797570850202"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="4.39271255060729"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,7 +1022,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1028,6 +1034,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
       <c r="B1" s="0"/>
       <c r="C1" s="1" t="s">
         <v>52</v>
@@ -1055,6 +1062,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0"/>
       <c r="B2" s="0"/>
       <c r="C2" s="1" t="n">
         <v>6</v>
@@ -1264,17 +1272,19 @@
       <c r="H8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="0"/>
+      <c r="I8" s="0" t="s">
+        <v>69</v>
+      </c>
       <c r="J8" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
@@ -1283,7 +1293,7 @@
         <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>43</v>
@@ -1294,26 +1304,28 @@
       <c r="H9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="0"/>
+      <c r="I9" s="0" t="s">
+        <v>73</v>
+      </c>
       <c r="J9" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>42</v>

</xml_diff>